<commit_message>
Update KETCHUP code and examples
</commit_message>
<xml_diff>
--- a/KETCHUP_main/example/data/FDH_model.xlsx
+++ b/KETCHUP_main/example/data/FDH_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjack\DOCUME~1\MobaXterm\slash\RemoteFiles\527074_2_2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pfs13/Documents/od/downloads 2025-10-01/KETCHUP v01/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F8034F-D27A-458B-8EBA-D57A8F9AE24C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D36AB989-5600-F945-B639-F299A86441A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="3840" windowWidth="17220" windowHeight="14865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="60" yWindow="3840" windowWidth="17220" windowHeight="14860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reactions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Rxn ID</t>
   </si>
@@ -104,6 +104,12 @@
   </si>
   <si>
     <t>(1) nad + (1) hco2 &lt;=&gt;  (1) nadh + (1) co2</t>
+  </si>
+  <si>
+    <t>fdh</t>
+  </si>
+  <si>
+    <t>Enzyme ID</t>
   </si>
 </sst>
 </file>
@@ -146,7 +152,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -169,17 +175,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -485,23 +505,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="53" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
     <col min="4" max="4" width="12" customWidth="1"/>
-    <col min="5" max="7" width="13.5703125" customWidth="1"/>
-    <col min="8" max="8" width="21.28515625" customWidth="1"/>
+    <col min="5" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +546,11 @@
       <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -552,8 +575,11 @@
       <c r="H2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -594,14 +620,14 @@
       <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" customWidth="1"/>
-    <col min="2" max="2" width="58.42578125" customWidth="1"/>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" customWidth="1"/>
+    <col min="2" max="2" width="58.5" customWidth="1"/>
+    <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -612,22 +638,22 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>21</v>
       </c>

</xml_diff>